<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Wed Jun 11 14:26:46 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-11 16:58:40 +0530</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-11 15:50:29 +0530</t>
+          <t>2025-06-11 16:58:40 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:50:29 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:02 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:02 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-10 10:28:13 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 10:28:13 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-05-30 15:24:23 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 15:24:23 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-05-28 01:32:38 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-28 01:32:38 +0530</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 17:24:03 +0530</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-16 19:21:06 +0530</t>
+          <t>2025-05-19 14:20:37 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-16 19:17:02 +0530</t>
+          <t>2025-05-16 19:21:06 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-16 18:10:55 +0530</t>
+          <t>2025-05-16 19:17:02 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-16 18:06:10 +0530</t>
+          <t>2025-05-16 18:10:55 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-16 17:23:21 +0530</t>
+          <t>2025-05-16 18:06:10 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-16 17:21:04 +0530</t>
+          <t>2025-05-16 17:23:21 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-16 17:18:57 +0530</t>
+          <t>2025-05-16 17:21:04 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-16 17:14:48 +0530</t>
+          <t>2025-05-16 17:18:57 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1990,17 +1990,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-16 16:41:42 +0530</t>
+          <t>2025-05-16 17:14:48 +0530</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2015,17 +2015,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-05-16 16:23:08 +0530</t>
+          <t>2025-05-16 16:41:42 +0530</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2040,17 +2040,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-04-15 17:02:19 +0530</t>
+          <t>2025-05-16 16:23:08 +0530</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2065,17 +2065,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-03-18 15:00:14 +0530</t>
+          <t>2025-04-15 17:02:19 +0530</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2090,17 +2090,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-03-11 20:14:25 +0530</t>
+          <t>2025-03-18 15:00:14 +0530</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2115,23 +2115,48 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2025-03-11 20:14:25 +0530</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Root</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="B69" t="inlineStr">
         <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>2025-03-11 17:39:36 +0530</t>
         </is>
       </c>
-      <c r="D68" t="n">
-        <v>1</v>
-      </c>
-      <c r="E68" t="inlineStr">
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" t="inlineStr">
         <is>
           <t>Root</t>
         </is>
@@ -2188,7 +2213,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-11 13:39:36 UTC</t>
+          <t>2025-06-11 14:26:46 UTC</t>
         </is>
       </c>
     </row>
@@ -2199,7 +2224,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5">
@@ -2210,7 +2235,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2252,7 +2277,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3">
@@ -2262,7 +2287,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
@@ -2283,7 +2308,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-11 16:58:40 +0530</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Wed Jun 11 14:41:31 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2201,7 +2201,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
+          <t>supreethr23/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-11 14:26:46 UTC</t>
+          <t>2025-06-11 14:41:31 UTC</t>
         </is>
       </c>
     </row>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Wed Jun 11 14:47:06 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-11 16:58:40 +0530</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-11 15:50:29 +0530</t>
+          <t>2025-06-11 16:58:40 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:50:29 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:02 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:02 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-10 10:28:13 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 10:28:13 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-05-30 15:24:23 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 15:24:23 +0530</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-05-28 01:32:38 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-28 01:32:38 +0530</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 17:24:03 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-16 19:21:06 +0530</t>
+          <t>2025-05-19 14:20:37 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-16 19:17:02 +0530</t>
+          <t>2025-05-16 19:21:06 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-16 18:10:55 +0530</t>
+          <t>2025-05-16 19:17:02 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-16 18:06:10 +0530</t>
+          <t>2025-05-16 18:10:55 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-16 17:23:21 +0530</t>
+          <t>2025-05-16 18:06:10 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-16 17:21:04 +0530</t>
+          <t>2025-05-16 17:23:21 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-16 17:18:57 +0530</t>
+          <t>2025-05-16 17:21:04 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1990,17 +1990,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-16 17:14:48 +0530</t>
+          <t>2025-05-16 17:18:57 +0530</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2015,17 +2015,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-05-16 16:41:42 +0530</t>
+          <t>2025-05-16 17:14:48 +0530</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2040,17 +2040,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-05-16 16:23:08 +0530</t>
+          <t>2025-05-16 16:41:42 +0530</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2065,17 +2065,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-04-15 17:02:19 +0530</t>
+          <t>2025-05-16 16:23:08 +0530</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2090,17 +2090,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-03-18 15:00:14 +0530</t>
+          <t>2025-04-15 17:02:19 +0530</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2115,17 +2115,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-03-11 20:14:25 +0530</t>
+          <t>2025-03-18 15:00:14 +0530</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2140,23 +2140,48 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>2025-03-11 20:14:25 +0530</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Root</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B70" t="inlineStr">
         <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C70" t="inlineStr">
         <is>
           <t>2025-03-11 17:39:36 +0530</t>
         </is>
       </c>
-      <c r="D69" t="n">
-        <v>1</v>
-      </c>
-      <c r="E69" t="inlineStr">
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" t="inlineStr">
         <is>
           <t>Root</t>
         </is>
@@ -2213,7 +2238,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-11 14:41:31 UTC</t>
+          <t>2025-06-11 14:47:06 UTC</t>
         </is>
       </c>
     </row>
@@ -2224,7 +2249,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5">
@@ -2235,7 +2260,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2302,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3">
@@ -2287,7 +2312,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4">
@@ -2308,7 +2333,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Wed Jun 11 14:50:01 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2226,7 +2226,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>supreethr23/MS-Innovation-Release-Notes</t>
+          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2238,7 +2238,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-11 14:47:06 UTC</t>
+          <t>2025-06-11 14:50:01 UTC</t>
         </is>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Wed Jun 11 15:41:19 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-11 16:58:40 +0530</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-11 15:50:29 +0530</t>
+          <t>2025-06-11 16:58:40 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:50:29 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:02 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:02 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-10 10:28:13 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 10:28:13 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-05-30 15:24:23 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-11 14:50:01 UTC</t>
+          <t>2025-06-11 15:41:19 UTC</t>
         </is>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Wed Jun 11 15:42:53 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:02 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:02 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-10 10:28:13 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 10:28:13 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-05-28 01:32:38 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-28 01:32:38 +0530</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 17:24:03 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-16 19:21:06 +0530</t>
+          <t>2025-05-19 14:20:37 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-16 19:17:02 +0530</t>
+          <t>2025-05-16 19:21:06 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-16 18:10:55 +0530</t>
+          <t>2025-05-16 19:17:02 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-16 18:06:10 +0530</t>
+          <t>2025-05-16 18:10:55 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-16 17:23:21 +0530</t>
+          <t>2025-05-16 18:06:10 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-16 17:21:04 +0530</t>
+          <t>2025-05-16 17:23:21 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1990,17 +1990,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-16 17:18:57 +0530</t>
+          <t>2025-05-16 17:21:04 +0530</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2015,17 +2015,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-05-16 17:14:48 +0530</t>
+          <t>2025-05-16 17:18:57 +0530</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2040,17 +2040,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-05-16 16:41:42 +0530</t>
+          <t>2025-05-16 17:14:48 +0530</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2065,17 +2065,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-05-16 16:23:08 +0530</t>
+          <t>2025-05-16 16:41:42 +0530</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2090,17 +2090,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-04-15 17:02:19 +0530</t>
+          <t>2025-05-16 16:23:08 +0530</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2115,17 +2115,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-03-18 15:00:14 +0530</t>
+          <t>2025-04-15 17:02:19 +0530</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2140,17 +2140,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-03-11 20:14:25 +0530</t>
+          <t>2025-03-18 15:00:14 +0530</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2165,23 +2165,48 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2025-03-11 20:14:25 +0530</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Root</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="B71" t="inlineStr">
         <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t>2025-03-11 17:39:36 +0530</t>
         </is>
       </c>
-      <c r="D70" t="n">
-        <v>1</v>
-      </c>
-      <c r="E70" t="inlineStr">
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" t="inlineStr">
         <is>
           <t>Root</t>
         </is>
@@ -2238,7 +2263,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-11 15:41:19 UTC</t>
+          <t>2025-06-11 15:42:53 UTC</t>
         </is>
       </c>
     </row>
@@ -2249,7 +2274,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
@@ -2260,7 +2285,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -2302,7 +2327,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3">
@@ -2312,7 +2337,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Wed Jun 11 16:53:46 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2251,7 +2251,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
+          <t>supreethr23/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-11 15:42:53 UTC</t>
+          <t>2025-06-11 16:53:45 UTC</t>
         </is>
       </c>
     </row>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Wed Jun 11 17:17:21 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -465,21 +465,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-11 16:58:40 +0530</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-11 15:50:29 +0530</t>
+          <t>2025-06-11 16:58:40 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 15:50:29 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:02 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:02 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-10 10:28:13 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-11 16:53:45 UTC</t>
+          <t>2025-06-11 17:17:20 UTC</t>
         </is>
       </c>
     </row>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -2358,7 +2358,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Wed Jun 11 17:20:34 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2251,7 +2251,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>supreethr23/MS-Innovation-Release-Notes</t>
+          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-11 17:17:20 UTC</t>
+          <t>2025-06-11 17:20:34 UTC</t>
         </is>
       </c>
     </row>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 06:48:45 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -465,21 +465,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -490,21 +490,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-11 16:58:40 +0530</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-11 15:50:29 +0530</t>
+          <t>2025-06-11 16:58:40 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 15:50:29 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:02 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-11 17:20:34 UTC</t>
+          <t>2025-06-12 06:48:45 UTC</t>
         </is>
       </c>
     </row>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
     </row>
@@ -2358,7 +2358,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 07:06:08 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,21 +490,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -515,21 +515,21 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-11 16:58:40 +0530</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-11 15:50:29 +0530</t>
+          <t>2025-06-11 16:58:40 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 06:48:45 UTC</t>
+          <t>2025-06-12 07:06:08 UTC</t>
         </is>
       </c>
     </row>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -2358,7 +2358,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 09:49:46 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,21 +515,21 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,21 +565,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-11 16:58:40 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-05-28 01:32:38 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-28 01:32:38 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 17:24:03 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-16 19:21:06 +0530</t>
+          <t>2025-05-19 14:20:37 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-16 19:17:02 +0530</t>
+          <t>2025-05-16 19:21:06 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-16 18:10:55 +0530</t>
+          <t>2025-05-16 19:17:02 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-16 18:06:10 +0530</t>
+          <t>2025-05-16 18:10:55 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-16 17:23:21 +0530</t>
+          <t>2025-05-16 18:06:10 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1990,17 +1990,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-16 17:21:04 +0530</t>
+          <t>2025-05-16 17:23:21 +0530</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2015,17 +2015,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-05-16 17:18:57 +0530</t>
+          <t>2025-05-16 17:21:04 +0530</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2040,17 +2040,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-05-16 17:14:48 +0530</t>
+          <t>2025-05-16 17:18:57 +0530</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2065,17 +2065,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-05-16 16:41:42 +0530</t>
+          <t>2025-05-16 17:14:48 +0530</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2090,17 +2090,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-05-16 16:23:08 +0530</t>
+          <t>2025-05-16 16:41:42 +0530</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2115,17 +2115,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-04-15 17:02:19 +0530</t>
+          <t>2025-05-16 16:23:08 +0530</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2140,17 +2140,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-03-18 15:00:14 +0530</t>
+          <t>2025-04-15 17:02:19 +0530</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2165,17 +2165,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2025-03-11 20:14:25 +0530</t>
+          <t>2025-03-18 15:00:14 +0530</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -2190,23 +2190,48 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>2025-03-11 20:14:25 +0530</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Root</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B72" t="inlineStr">
         <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>2025-03-11 17:39:36 +0530</t>
         </is>
       </c>
-      <c r="D71" t="n">
-        <v>1</v>
-      </c>
-      <c r="E71" t="inlineStr">
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" t="inlineStr">
         <is>
           <t>Root</t>
         </is>
@@ -2263,7 +2288,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 07:06:08 UTC</t>
+          <t>2025-06-12 09:49:46 UTC</t>
         </is>
       </c>
     </row>
@@ -2274,7 +2299,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
@@ -2285,7 +2310,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -2327,7 +2352,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
@@ -2337,7 +2362,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
@@ -2358,7 +2383,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 10:24:13 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2276,7 +2276,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
+          <t>Riya10031/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 09:49:46 UTC</t>
+          <t>2025-06-12 10:24:13 UTC</t>
         </is>
       </c>
     </row>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 10:29:52 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,12 +490,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,21 +565,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -590,21 +590,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-05-28 01:32:38 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-28 01:32:38 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 17:24:03 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-16 19:21:06 +0530</t>
+          <t>2025-05-19 14:20:37 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-16 19:17:02 +0530</t>
+          <t>2025-05-16 19:21:06 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-16 18:10:55 +0530</t>
+          <t>2025-05-16 19:17:02 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-16 18:06:10 +0530</t>
+          <t>2025-05-16 18:10:55 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -2288,7 +2288,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 10:24:13 UTC</t>
+          <t>2025-06-12 10:29:52 UTC</t>
         </is>
       </c>
     </row>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2383,7 +2383,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 10:36:39 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -490,12 +490,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -515,12 +515,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Riya10031/MS-Innovation-Release-Notes</t>
+          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 10:29:52 UTC</t>
+          <t>2025-06-12 10:36:39 UTC</t>
         </is>
       </c>
     </row>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 11:08:10 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 15:59:35 +0530</t>
+          <t>2025-06-12 16:16:30 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,12 +515,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,21 +590,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -615,21 +615,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-05-28 01:32:38 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-28 01:32:38 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 17:24:03 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-16 19:21:06 +0530</t>
+          <t>2025-05-19 14:20:37 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-16 19:17:02 +0530</t>
+          <t>2025-05-16 19:21:06 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-16 18:10:55 +0530</t>
+          <t>2025-05-16 19:17:02 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1990,17 +1990,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-16 17:23:21 +0530</t>
+          <t>2025-05-16 18:10:55 +0530</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2015,17 +2015,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-05-16 17:21:04 +0530</t>
+          <t>2025-05-16 17:23:21 +0530</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2040,17 +2040,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-05-16 17:18:57 +0530</t>
+          <t>2025-05-16 17:21:04 +0530</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2065,17 +2065,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-05-16 17:14:48 +0530</t>
+          <t>2025-05-16 17:18:57 +0530</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2090,17 +2090,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-05-16 16:41:42 +0530</t>
+          <t>2025-05-16 17:14:48 +0530</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2115,17 +2115,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-05-16 16:23:08 +0530</t>
+          <t>2025-05-16 16:41:42 +0530</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2140,17 +2140,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-04-15 17:02:19 +0530</t>
+          <t>2025-05-16 16:23:08 +0530</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2165,17 +2165,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2025-03-18 15:00:14 +0530</t>
+          <t>2025-04-15 17:02:19 +0530</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -2190,17 +2190,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2025-03-11 20:14:25 +0530</t>
+          <t>2025-03-18 15:00:14 +0530</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2215,23 +2215,48 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2025-03-11 20:14:25 +0530</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Root</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="B73" t="inlineStr">
         <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="C73" t="inlineStr">
         <is>
           <t>2025-03-11 17:39:36 +0530</t>
         </is>
       </c>
-      <c r="D72" t="n">
-        <v>1</v>
-      </c>
-      <c r="E72" t="inlineStr">
+      <c r="D73" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" t="inlineStr">
         <is>
           <t>Root</t>
         </is>
@@ -2288,7 +2313,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 10:36:39 UTC</t>
+          <t>2025-06-12 11:08:10 UTC</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2324,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
@@ -2310,7 +2335,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
     </row>
@@ -2352,7 +2377,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
@@ -2362,7 +2387,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
@@ -2383,7 +2408,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 15:59:35 +0530</t>
+          <t>2025-06-12 16:16:30 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 11:56:38 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 16:16:30 +0530</t>
+          <t>2025-06-12 17:26:19 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-12 15:59:35 +0530</t>
+          <t>2025-06-12 16:16:30 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,12 +540,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,21 +615,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -640,21 +640,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-05-28 01:32:38 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-28 01:32:38 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 17:24:03 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-16 19:21:06 +0530</t>
+          <t>2025-05-19 14:20:37 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-16 19:17:02 +0530</t>
+          <t>2025-05-16 19:21:06 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1990,17 +1990,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-16 18:10:55 +0530</t>
+          <t>2025-05-16 19:17:02 +0530</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2015,17 +2015,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-05-16 17:23:21 +0530</t>
+          <t>2025-05-16 18:10:55 +0530</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2040,17 +2040,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-05-16 17:21:04 +0530</t>
+          <t>2025-05-16 17:23:21 +0530</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2065,17 +2065,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-05-16 17:18:57 +0530</t>
+          <t>2025-05-16 17:21:04 +0530</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2090,17 +2090,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-05-16 17:14:48 +0530</t>
+          <t>2025-05-16 17:18:57 +0530</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2115,17 +2115,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-05-16 16:41:42 +0530</t>
+          <t>2025-05-16 17:14:48 +0530</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2140,17 +2140,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-05-16 16:23:08 +0530</t>
+          <t>2025-05-16 16:41:42 +0530</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2165,17 +2165,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2025-04-15 17:02:19 +0530</t>
+          <t>2025-05-16 16:23:08 +0530</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -2190,17 +2190,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2025-03-18 15:00:14 +0530</t>
+          <t>2025-04-15 17:02:19 +0530</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2215,17 +2215,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2025-03-11 20:14:25 +0530</t>
+          <t>2025-03-18 15:00:14 +0530</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2240,23 +2240,48 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>2025-03-11 20:14:25 +0530</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Root</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B74" t="inlineStr">
         <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C74" t="inlineStr">
         <is>
           <t>2025-03-11 17:39:36 +0530</t>
         </is>
       </c>
-      <c r="D73" t="n">
-        <v>1</v>
-      </c>
-      <c r="E73" t="inlineStr">
+      <c r="D74" t="n">
+        <v>1</v>
+      </c>
+      <c r="E74" t="inlineStr">
         <is>
           <t>Root</t>
         </is>
@@ -2313,7 +2338,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 11:08:10 UTC</t>
+          <t>2025-06-12 11:56:38 UTC</t>
         </is>
       </c>
     </row>
@@ -2324,7 +2349,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
@@ -2335,7 +2360,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
     </row>
@@ -2377,7 +2402,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3">
@@ -2387,7 +2412,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4">
@@ -2408,7 +2433,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 16:16:30 +0530</t>
+          <t>2025-06-12 17:26:19 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 12:04:26 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 17:26:19 +0530</t>
+          <t>2025-06-12 17:31:45 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-12 16:16:30 +0530</t>
+          <t>2025-06-12 17:26:19 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-12 15:59:35 +0530</t>
+          <t>2025-06-12 16:16:30 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 11:56:38 UTC</t>
+          <t>2025-06-12 12:04:26 UTC</t>
         </is>
       </c>
     </row>
@@ -2360,7 +2360,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
     </row>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 17:26:19 +0530</t>
+          <t>2025-06-12 17:31:45 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 12:07:04 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -475,7 +475,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 17:31:45 +0530</t>
+          <t>2025-06-12 17:36:45 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 12:04:26 UTC</t>
+          <t>2025-06-12 12:07:04 UTC</t>
         </is>
       </c>
     </row>
@@ -2360,7 +2360,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
     </row>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 17:31:45 +0530</t>
+          <t>2025-06-12 17:36:45 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 12:07:25 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -475,7 +475,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 17:36:45 +0530</t>
+          <t>2025-06-12 17:37:08 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 12:07:04 UTC</t>
+          <t>2025-06-12 12:07:25 UTC</t>
         </is>
       </c>
     </row>
@@ -2360,7 +2360,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
     </row>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 17:36:45 +0530</t>
+          <t>2025-06-12 17:37:08 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 14:03:54 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 13:14:34 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,21 +640,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -665,21 +665,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-28 01:32:38 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-28 01:32:38 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 17:24:03 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-16 19:21:06 +0530</t>
+          <t>2025-05-19 14:20:37 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1990,17 +1990,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-16 19:17:02 +0530</t>
+          <t>2025-05-16 19:21:06 +0530</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2015,17 +2015,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-05-16 18:10:55 +0530</t>
+          <t>2025-05-16 19:17:02 +0530</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2040,17 +2040,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-05-16 17:23:21 +0530</t>
+          <t>2025-05-16 18:10:55 +0530</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2065,17 +2065,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-05-16 17:21:04 +0530</t>
+          <t>2025-05-16 17:23:21 +0530</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2090,17 +2090,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-05-16 17:18:57 +0530</t>
+          <t>2025-05-16 17:21:04 +0530</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2115,17 +2115,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-05-16 17:14:48 +0530</t>
+          <t>2025-05-16 17:18:57 +0530</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2140,17 +2140,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-05-16 16:41:42 +0530</t>
+          <t>2025-05-16 17:14:48 +0530</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2165,17 +2165,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2025-05-16 16:23:08 +0530</t>
+          <t>2025-05-16 16:41:42 +0530</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -2190,17 +2190,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2025-04-15 17:02:19 +0530</t>
+          <t>2025-05-16 16:23:08 +0530</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2215,17 +2215,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2025-03-18 15:00:14 +0530</t>
+          <t>2025-04-15 17:02:19 +0530</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2240,17 +2240,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2025-03-11 20:14:25 +0530</t>
+          <t>2025-03-18 15:00:14 +0530</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -2265,23 +2265,48 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>2025-03-11 20:14:25 +0530</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>1</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Root</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B75" t="inlineStr">
         <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C75" t="inlineStr">
         <is>
           <t>2025-03-11 17:39:36 +0530</t>
         </is>
       </c>
-      <c r="D74" t="n">
-        <v>1</v>
-      </c>
-      <c r="E74" t="inlineStr">
+      <c r="D75" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" t="inlineStr">
         <is>
           <t>Root</t>
         </is>
@@ -2338,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 12:07:25 UTC</t>
+          <t>2025-06-12 14:03:54 UTC</t>
         </is>
       </c>
     </row>
@@ -2349,7 +2374,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
@@ -2360,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
     </row>
@@ -2402,7 +2427,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
@@ -2412,7 +2437,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 15:25:18 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 17:37:08 +0530</t>
+          <t>2025-06-12 20:05:46 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-12 17:26:19 +0530</t>
+          <t>2025-06-12 17:37:08 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-12 16:16:30 +0530</t>
+          <t>2025-06-12 17:26:19 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-12 15:59:35 +0530</t>
+          <t>2025-06-12 16:16:30 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-12 13:14:34 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 13:14:34 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,21 +665,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -690,21 +690,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-28 01:32:38 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-28 01:32:38 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 17:24:03 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1990,17 +1990,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-16 19:21:06 +0530</t>
+          <t>2025-05-19 14:20:37 +0530</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2015,17 +2015,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-05-16 19:17:02 +0530</t>
+          <t>2025-05-16 19:21:06 +0530</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2040,17 +2040,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-05-16 18:10:55 +0530</t>
+          <t>2025-05-16 19:17:02 +0530</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 14:03:54 UTC</t>
+          <t>2025-06-12 15:25:18 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
         </is>
       </c>
     </row>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 17:37:08 +0530</t>
+          <t>2025-06-12 20:05:46 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 16:17:24 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2351,7 +2351,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
+          <t>supreethr23/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 15:25:18 UTC</t>
+          <t>2025-06-12 16:17:24 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 16:20:02 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 20:05:46 +0530</t>
+          <t>2025-06-12 21:49:46 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-12 17:37:08 +0530</t>
+          <t>2025-06-12 20:05:46 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-12 17:26:19 +0530</t>
+          <t>2025-06-12 17:37:08 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-12 16:16:30 +0530</t>
+          <t>2025-06-12 17:26:19 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-12 15:59:35 +0530</t>
+          <t>2025-06-12 16:16:30 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-12 13:14:34 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 13:14:34 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,21 +690,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -715,21 +715,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -740,17 +740,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-28 01:32:38 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 16:17:24 UTC</t>
+          <t>2025-06-12 16:20:02 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 20:05:46 +0530</t>
+          <t>2025-06-12 21:49:46 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 16:20:33 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -475,7 +475,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 21:49:46 +0530</t>
+          <t>2025-06-12 21:50:14 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 16:20:02 UTC</t>
+          <t>2025-06-12 16:20:33 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
     </row>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 21:49:46 +0530</t>
+          <t>2025-06-12 21:50:14 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Thu Jun 12 16:56:13 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2351,7 +2351,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>supreethr23/MS-Innovation-Release-Notes</t>
+          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 16:20:33 UTC</t>
+          <t>2025-06-12 16:56:13 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>18</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 07:25:48 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2351,7 +2351,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
+          <t>Prapthi564/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 16:56:13 UTC</t>
+          <t>2025-06-13 07:25:48 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 07:31:54 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-12 21:50:14 +0530</t>
+          <t>2025-06-13 13:01:36 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-12 20:05:46 +0530</t>
+          <t>2025-06-12 21:50:14 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-12 17:37:08 +0530</t>
+          <t>2025-06-12 20:05:46 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-12 17:26:19 +0530</t>
+          <t>2025-06-12 17:37:08 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-12 16:16:30 +0530</t>
+          <t>2025-06-12 17:26:19 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-12 15:59:35 +0530</t>
+          <t>2025-06-12 16:16:30 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-12 13:14:34 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 07:25:48 UTC</t>
+          <t>2025-06-13 07:31:54 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-12 21:50:14 +0530</t>
+          <t>2025-06-13 13:01:36 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 07:37:07 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -475,7 +475,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-13 13:01:36 +0530</t>
+          <t>2025-06-13 13:06:50 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 07:31:54 UTC</t>
+          <t>2025-06-13 07:37:07 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-13 13:01:36 +0530</t>
+          <t>2025-06-13 13:06:50 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 07:39:05 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
+          <t>Developing_a_Custom_RAG_App_Using_Azure_AI_Foundry</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
+          <t>Developing_a_Custom_RAG_App_Using_Azure_AI_Foundry</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-13 13:06:50 +0530</t>
+          <t>2025-06-13 13:08:47 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-12 21:50:14 +0530</t>
+          <t>2025-06-13 13:06:50 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-12 20:05:46 +0530</t>
+          <t>2025-06-12 21:50:14 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-12 17:37:08 +0530</t>
+          <t>2025-06-12 20:05:46 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-12 17:26:19 +0530</t>
+          <t>2025-06-12 17:37:08 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-12 16:16:30 +0530</t>
+          <t>2025-06-12 17:26:19 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-12 15:59:35 +0530</t>
+          <t>2025-06-12 16:16:30 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,21 +715,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -740,21 +740,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 17:24:03 +0530</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1990,17 +1990,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2015,17 +2015,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-05-16 19:21:06 +0530</t>
+          <t>2025-05-19 14:20:37 +0530</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2040,17 +2040,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-05-16 19:17:02 +0530</t>
+          <t>2025-05-16 19:21:06 +0530</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2065,17 +2065,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-05-16 17:23:21 +0530</t>
+          <t>2025-05-16 19:17:02 +0530</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2090,17 +2090,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-05-16 17:21:04 +0530</t>
+          <t>2025-05-16 17:23:21 +0530</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2115,17 +2115,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-05-16 17:18:57 +0530</t>
+          <t>2025-05-16 17:21:04 +0530</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2140,17 +2140,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-05-16 17:14:48 +0530</t>
+          <t>2025-05-16 17:18:57 +0530</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2165,17 +2165,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2025-05-16 16:41:42 +0530</t>
+          <t>2025-05-16 17:14:48 +0530</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -2190,17 +2190,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2025-05-16 16:23:08 +0530</t>
+          <t>2025-05-16 16:41:42 +0530</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2215,17 +2215,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2025-04-15 17:02:19 +0530</t>
+          <t>2025-05-16 16:23:08 +0530</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2240,17 +2240,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2025-03-18 15:00:14 +0530</t>
+          <t>2025-04-15 17:02:19 +0530</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -2265,17 +2265,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2025-03-11 20:14:25 +0530</t>
+          <t>2025-03-18 15:00:14 +0530</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -2290,23 +2290,48 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Real-time Analytics with Synapse</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2025-03-11 20:14:25 +0530</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Root</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
+      <c r="B76" t="inlineStr">
         <is>
           <t>Power BI Embedded</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="C76" t="inlineStr">
         <is>
           <t>2025-03-11 17:39:36 +0530</t>
         </is>
       </c>
-      <c r="D75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E75" t="inlineStr">
+      <c r="D76" t="n">
+        <v>1</v>
+      </c>
+      <c r="E76" t="inlineStr">
         <is>
           <t>Root</t>
         </is>
@@ -2363,7 +2388,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 07:37:07 UTC</t>
+          <t>2025-06-13 07:39:05 UTC</t>
         </is>
       </c>
     </row>
@@ -2374,7 +2399,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -2385,7 +2410,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -2427,7 +2452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
@@ -2437,7 +2462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4">
@@ -2458,7 +2483,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-13 13:06:50 +0530</t>
+          <t>2025-06-13 13:08:47 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 07:39:58 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -475,7 +475,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-13 13:08:47 +0530</t>
+          <t>2025-06-13 13:09:40 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -2388,7 +2388,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 07:39:05 UTC</t>
+          <t>2025-06-13 07:39:57 UTC</t>
         </is>
       </c>
     </row>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-13 13:08:47 +0530</t>
+          <t>2025-06-13 13:09:40 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 07:41:24 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2376,7 +2376,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Prapthi564/MS-Innovation-Release-Notes</t>
+          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 07:39:57 UTC</t>
+          <t>2025-06-13 07:41:24 UTC</t>
         </is>
       </c>
     </row>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>19</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 07:47:12 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Build-Custom-Knowledge-RAG-App-With-Azure-AI-Foundry</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-13 13:06:50 +0530</t>
+          <t>2025-06-12 21:50:14 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-12 21:50:14 +0530</t>
+          <t>2025-06-12 20:05:46 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-12 20:05:46 +0530</t>
+          <t>2025-06-12 17:37:08 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-12 17:37:08 +0530</t>
+          <t>2025-06-12 17:26:19 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-12 17:26:19 +0530</t>
+          <t>2025-06-12 16:16:30 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-12 16:16:30 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-12 15:59:35 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,21 +715,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -740,21 +740,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-27 17:24:03 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1990,17 +1990,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-19 14:20:37 +0530</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2015,17 +2015,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Hackathon - Microsoft Azure OpenHack</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-16 19:21:06 +0530</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -2040,17 +2040,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Hackathon - Microsoft Azure OpenHack</t>
+          <t>Azure Red Hat OpenShift Workshop</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2025-05-16 19:21:06 +0530</t>
+          <t>2025-05-16 19:17:02 +0530</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -2065,17 +2065,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Azure Red Hat OpenShift Workshop</t>
+          <t>Building a Resilient IaaS Architecture</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2025-05-16 19:17:02 +0530</t>
+          <t>2025-05-16 17:23:21 +0530</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -2090,17 +2090,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Building a Resilient IaaS Architecture</t>
+          <t>​Azure API Management</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2025-05-16 17:23:21 +0530</t>
+          <t>2025-05-16 17:21:04 +0530</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -2115,17 +2115,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>​Azure API Management</t>
+          <t>Code Suggestions with GitHub Copilot in VS Code</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2025-05-16 17:21:04 +0530</t>
+          <t>2025-05-16 17:18:57 +0530</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2140,17 +2140,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in VS Code</t>
+          <t>Securing Repositories with GitHub Advanced Security</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2025-05-16 17:18:57 +0530</t>
+          <t>2025-05-16 17:14:48 +0530</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -2165,17 +2165,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Securing Repositories with GitHub Advanced Security</t>
+          <t>Hackathon - Introduction to Building AI Apps</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2025-05-16 17:14:48 +0530</t>
+          <t>2025-05-16 16:41:42 +0530</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -2190,17 +2190,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Hackathon - Introduction to Building AI Apps</t>
+          <t>Fabric-Analytics-in-aday</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2025-05-16 16:41:42 +0530</t>
+          <t>2025-05-16 16:23:08 +0530</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -2215,17 +2215,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Fabric-Analytics-in-aday</t>
+          <t>LLM-Ops-Hands-On-lab</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2025-05-16 16:23:08 +0530</t>
+          <t>2025-04-15 17:02:19 +0530</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -2240,17 +2240,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>LLM-Ops-Hands-On-lab</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2025-04-15 17:02:19 +0530</t>
+          <t>2025-03-18 15:00:14 +0530</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -2265,17 +2265,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>Real-time Analytics with Synapse</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Format</t>
+          <t>Real-time Analytics with Synapse</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2025-03-18 15:00:14 +0530</t>
+          <t>2025-03-11 20:14:25 +0530</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -2290,48 +2290,23 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Power BI Embedded</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Real-time Analytics with Synapse</t>
+          <t>Power BI Embedded</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2025-03-11 20:14:25 +0530</t>
+          <t>2025-03-11 17:39:36 +0530</t>
         </is>
       </c>
       <c r="D75" t="n">
         <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
-        <is>
-          <t>Root</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Power BI Embedded</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Power BI Embedded</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>2025-03-11 17:39:36 +0530</t>
-        </is>
-      </c>
-      <c r="D76" t="n">
-        <v>1</v>
-      </c>
-      <c r="E76" t="inlineStr">
         <is>
           <t>Root</t>
         </is>
@@ -2388,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 07:41:24 UTC</t>
+          <t>2025-06-13 07:47:12 UTC</t>
         </is>
       </c>
     </row>
@@ -2399,7 +2374,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5">
@@ -2410,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>20</t>
         </is>
       </c>
     </row>
@@ -2452,7 +2427,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
@@ -2462,7 +2437,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 12:05:27 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2351,7 +2351,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
+          <t>sachinym/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 07:47:12 UTC</t>
+          <t>2025-06-13 12:05:27 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 12:06:07 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -465,17 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Developing_a_Custom_RAG_App_Using_Azure_AI_Foundry</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Developing_a_Custom_RAG_App_Using_Azure_AI_Foundry</t>
+          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-06-13 13:09:40 +0530</t>
+          <t>2025-06-13 17:35:45 +0530</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t>Developing_a_Custom_RAG_App_Using_Azure_AI_Foundry</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t>Developing_a_Custom_RAG_App_Using_Azure_AI_Foundry</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-12 21:50:14 +0530</t>
+          <t>2025-06-13 13:09:40 +0530</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-12 20:05:46 +0530</t>
+          <t>2025-06-12 21:50:14 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-12 17:37:08 +0530</t>
+          <t>2025-06-12 20:05:46 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-12 17:26:19 +0530</t>
+          <t>2025-06-12 17:37:08 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-12 16:16:30 +0530</t>
+          <t>2025-06-12 17:26:19 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-12 15:59:35 +0530</t>
+          <t>2025-06-12 16:16:30 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,21 +715,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -740,21 +740,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -765,17 +765,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Azure_Well-Architected_Resiliency_Gaps_Remediation</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-27 17:24:03 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 12:05:27 UTC</t>
+          <t>2025-06-13 12:06:07 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-13 13:09:40 +0530</t>
+          <t>2025-06-13 17:35:45 +0530</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 13:19:30 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2351,7 +2351,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sachinym/MS-Innovation-Release-Notes</t>
+          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 12:06:07 UTC</t>
+          <t>2025-06-13 13:19:30 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>21</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 15:17:16 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2351,7 +2351,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CloudLabsAI-Azure/MS-Innovation-Release-Notes</t>
+          <t>shivamujawame/MS-Innovation-Release-Notes</t>
         </is>
       </c>
     </row>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 13:19:30 UTC</t>
+          <t>2025-06-13 15:17:16 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Fri Jun 13 15:19:23 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -490,17 +490,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Developing_a_Custom_RAG_App_Using_Azure_AI_Foundry</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Developing_a_Custom_RAG_App_Using_Azure_AI_Foundry</t>
+          <t>Implement CI-CD with GitHub Actions</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-06-13 13:09:40 +0530</t>
+          <t>2025-06-13 15:19:07 +0000</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -515,17 +515,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t>Developing_a_Custom_RAG_App_Using_Azure_AI_Foundry</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Automated Machine Learning Using AML</t>
+          <t>Developing_a_Custom_RAG_App_Using_Azure_AI_Foundry</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-06-12 21:50:14 +0530</t>
+          <t>2025-06-13 13:09:40 +0530</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -540,17 +540,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
+          <t>Automated Machine Learning Using AML</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-06-12 20:05:46 +0530</t>
+          <t>2025-06-12 21:50:14 +0530</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,17 +565,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Azure Virtual Machine And Compute</t>
+          <t>Create and Publish PowerBI Dashboards &amp; Reports</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-06-12 17:37:08 +0530</t>
+          <t>2025-06-12 20:05:46 +0530</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -590,17 +590,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
+          <t>Azure Virtual Machine And Compute</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-06-12 17:26:19 +0530</t>
+          <t>2025-06-12 17:37:08 +0530</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -615,17 +615,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
+          <t>Work with Data Lake and Data Factory Pipelines in Microsoft Fabric​</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-06-12 16:16:30 +0530</t>
+          <t>2025-06-12 17:26:19 +0530</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -640,17 +640,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
+          <t>Get Started with Microsoft Fabric with Its Lakehouses</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-06-12 15:59:35 +0530</t>
+          <t>2025-06-12 16:16:30 +0530</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -665,17 +665,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
+          <t>Build A Fabric Real-Time Intelligence Solution in a Day</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-06-12 15:19:27 +0530</t>
+          <t>2025-06-12 15:59:35 +0530</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -690,17 +690,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Enterprise-Class Networking in Azure</t>
+          <t>Azure_AI_Foundry_and_Semantic_Kernel_Fundamentals</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-06-12 12:35:48 +0530</t>
+          <t>2025-06-12 15:19:27 +0530</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -715,17 +715,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cloud-Native Applications</t>
+          <t>Enterprise-Class Networking in Azure</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-06-12 12:18:28 +0530</t>
+          <t>2025-06-12 12:35:48 +0530</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -740,21 +740,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hackathon - Activate GenAI with Azure</t>
+          <t>Cloud-Native Applications</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-06-11 22:47:04 +0530</t>
+          <t>2025-06-12 12:18:28 +0530</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -765,21 +765,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Azure Landing Zone</t>
+          <t>Hackathon - Activate GenAI with Azure</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-06-11 20:16:49 +0530</t>
+          <t>2025-06-11 22:47:04 +0530</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -790,17 +790,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Microsoft Azure AI Agents</t>
+          <t>Azure Landing Zone</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-06-11 20:13:48 +0530</t>
+          <t>2025-06-11 20:16:49 +0530</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -815,17 +815,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Azure Local Hands-on Lab</t>
+          <t>Microsoft Azure AI Agents</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2025-06-11 19:56:28 +0530</t>
+          <t>2025-06-11 20:13:48 +0530</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -840,17 +840,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Get data into Fabric Lakehouse</t>
+          <t>Azure Local Hands-on Lab</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00:50 +0000</t>
+          <t>2025-06-11 19:56:28 +0530</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -865,17 +865,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Low Code for Pro-Dev in a Day</t>
+          <t>Get data into Fabric Lakehouse</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2025-06-11 00:35:20 +0530</t>
+          <t>2025-06-11 15:00:50 +0000</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -890,17 +890,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Developing AI Applications with Azure AI Foundry</t>
+          <t>Low Code for Pro-Dev in a Day</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2025-06-11 00:33:06 +0530</t>
+          <t>2025-06-11 00:35:20 +0530</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -915,17 +915,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
+          <t>Developing AI Applications with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2025-06-10 23:22:30 +0530</t>
+          <t>2025-06-11 00:33:06 +0530</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -940,17 +940,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
+          <t>Develop Generative AI solutions with Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2025-06-10 23:10:36 +0530</t>
+          <t>2025-06-10 23:22:30 +0530</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -965,17 +965,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Get Started With OpenAI And Build Natural Language Solution</t>
+          <t xml:space="preserve">Advanced Workflow Automation with GitHub Actions </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2025-06-10 22:51:47 +0530</t>
+          <t>2025-06-10 23:10:36 +0530</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -990,17 +990,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
+          <t>Get Started With OpenAI And Build Natural Language Solution</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2025-06-10 22:48:16 +0530</t>
+          <t>2025-06-10 22:51:47 +0530</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1015,17 +1015,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
+          <t>Lunch and Learn: Building and Evaluating Prompt Flows with Azure AI Foundry</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2025-06-10 07:51:57 +0530</t>
+          <t>2025-06-10 22:48:16 +0530</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1040,17 +1040,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Azure Virtual Desktop</t>
+          <t>Automate document processing by using Azure AI &amp; OpenAI</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2025-06-09 23:17:02 +0530</t>
+          <t>2025-06-10 07:51:57 +0530</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1065,17 +1065,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
+          <t>Azure Virtual Desktop</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2025-06-09 18:18:42 +0530</t>
+          <t>2025-06-09 23:17:02 +0530</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1090,17 +1090,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
+          <t>Get Started with Real-Time Analytics and Data Science with Microsoft Fabric</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2025-06-09 17:15:52 +0530</t>
+          <t>2025-06-09 18:18:42 +0530</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1115,17 +1115,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
+          <t>Code Suggestions with GitHub Copilot in Codespace using VS Code</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2025-06-09 16:24:38 +0530</t>
+          <t>2025-06-09 17:15:52 +0530</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1140,17 +1140,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
+          <t>Customer Support Conversation Summarization with Azure OpenAI</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2025-06-09 14:20:04 +0000</t>
+          <t>2025-06-09 16:24:38 +0530</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1165,17 +1165,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Build Prompt Engineering With Azure OpenAI Service</t>
+          <t>Secure Windows Servers Azure Arc &amp; Microsoft Defender</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2025-06-05 22:32:54 +0530</t>
+          <t>2025-06-09 14:20:04 +0000</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1190,17 +1190,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
+          <t>Build Prompt Engineering With Azure OpenAI Service</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2025-06-05 21:53:26 +0530</t>
+          <t>2025-06-05 22:32:54 +0530</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1215,17 +1215,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Microsoft Fabric with capacity-copilot-SDP</t>
+          <t>Lunch and Learn: Build Custom Copilot Application using Azure AI Foundry</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2025-06-05 19:53:59 +0530</t>
+          <t>2025-06-05 21:53:26 +0530</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1240,17 +1240,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
+          <t>Microsoft Fabric with capacity-copilot-SDP</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:34 +0530</t>
+          <t>2025-06-05 19:53:59 +0530</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1265,17 +1265,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v2</t>
+          <t>Migrate-and-Modernise-SQL-Servers-to-Azure</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:20 +0530</t>
+          <t>2025-06-05 19:52:34 +0530</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1290,17 +1290,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Microsoft Defender for Cloud - v1</t>
+          <t>Microsoft Defender for Cloud - v2</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2025-06-05 19:52:09 +0530</t>
+          <t>2025-06-05 19:52:20 +0530</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1315,17 +1315,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Github&amp;AgenticAI</t>
+          <t>Microsoft Defender for Cloud - v1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2025-06-04 23:32:46 +0530</t>
+          <t>2025-06-05 19:52:09 +0530</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1340,17 +1340,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
+          <t>Github&amp;AgenticAI</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2025-06-04 17:43:54 +0300</t>
+          <t>2025-06-04 23:32:46 +0530</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1365,17 +1365,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Marketing</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2025-06-04 17:41:59 +0300</t>
+          <t>2025-06-04 17:43:54 +0300</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1390,17 +1390,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
+          <t>Leverage-Microsoft-365-Copilot-and-Copilot-Studio-for-Sales</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2025-06-04 17:37:32 +0300</t>
+          <t>2025-06-04 17:41:59 +0300</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1415,17 +1415,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
+          <t>Leverage-Microsoft365-Copilot-and-Copilot-Studio-for-Human-Resources</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2025-06-04 15:08:23 +0530</t>
+          <t>2025-06-04 17:37:32 +0300</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1440,17 +1440,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
+          <t>Use Azure Open AI Like A Pro To Build Powerful AI Applications</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2025-06-04 15:04:23 +0530</t>
+          <t>2025-06-04 15:08:23 +0530</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1465,17 +1465,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Fabric Copilot</t>
+          <t>Business Automation with Azure OpenAI and Document Intelligence</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2025-06-04 02:16:22 +0530</t>
+          <t>2025-06-04 15:04:23 +0530</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1490,17 +1490,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Integrate Azure OpenAI into your app</t>
+          <t>Fabric Copilot</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2025-06-03 13:54:36 +0530</t>
+          <t>2025-06-04 02:16:22 +0530</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1515,17 +1515,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
+          <t>Integrate Azure OpenAI into your app</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2025-05-30 20:59:44 +0530</t>
+          <t>2025-06-03 13:54:36 +0530</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1540,17 +1540,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>GitHub Copilot Innovation Workshop</t>
+          <t xml:space="preserve">Hackathon - GitHub Copilot </t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2025-05-30 18:54:48 +0530</t>
+          <t>2025-05-30 20:59:44 +0530</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1565,17 +1565,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
+          <t>GitHub Copilot Innovation Workshop</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2025-05-29 23:23:52 +0530</t>
+          <t>2025-05-30 18:54:48 +0530</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1590,17 +1590,17 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
+          <t xml:space="preserve">Call Center data analysis using Azure AI services and Azure OpenAI </t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2025-05-27 20:12:49 +0530</t>
+          <t>2025-05-29 23:23:52 +0530</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1615,17 +1615,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Power_Platform_Workshop:Administration_and_Governance</t>
+          <t>Hackathon - Intelligent App Development with Microsoft CoPilot Stack</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2025-05-27 14:48:39 +0530</t>
+          <t>2025-05-27 20:12:49 +0530</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1640,17 +1640,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Power Platform Workshop: Administration and Governance</t>
+          <t>Power_Platform_Workshop:Administration_and_Governance</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2025-05-27 07:23:52 +0000</t>
+          <t>2025-05-27 14:48:39 +0530</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1665,17 +1665,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Getting-started-with-Azure-OpenAI-services</t>
+          <t>Power Platform Workshop: Administration and Governance</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2025-05-26 20:28:36 +0530</t>
+          <t>2025-05-27 07:23:52 +0000</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1690,17 +1690,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Generate Code and Images with Azure OpenAI Services</t>
+          <t>Getting-started-with-Azure-OpenAI-services</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2025-05-26 18:35:30 +0530</t>
+          <t>2025-05-26 20:28:36 +0530</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1715,17 +1715,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Application Modernization 1 Day</t>
+          <t>Generate Code and Images with Azure OpenAI Services</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2025-05-26 14:28:12 +0530</t>
+          <t>2025-05-26 18:35:30 +0530</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1740,17 +1740,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Build Creative App using Azure AI and Prompty</t>
+          <t>Application Modernization 1 Day</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2025-05-24 22:26:24 +0530</t>
+          <t>2025-05-26 14:28:12 +0530</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1765,17 +1765,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
+          <t>Build Creative App using Azure AI and Prompty</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2025-05-24 22:25:09 +0530</t>
+          <t>2025-05-24 22:26:24 +0530</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1790,17 +1790,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Cloud Native Application Architecture</t>
+          <t>ADVANCED AZURE NETWORKING WITH AZURE VIRTUAL WAN(Azure Networking Solutions-301)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2025-05-23 19:32:21 +0530</t>
+          <t>2025-05-24 22:25:09 +0530</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1815,17 +1815,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
+          <t>Cloud Native Application Architecture</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2025-05-23 00:37:27 +0530</t>
+          <t>2025-05-23 19:32:21 +0530</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1840,17 +1840,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Hackathon - Accelerate Developer Productivity</t>
+          <t>Enterprise Knowledge Base Search and Query with Azure OpenAI and Azure AI Search</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2025-05-22 10:37:15 +0530</t>
+          <t>2025-05-23 00:37:27 +0530</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -1865,17 +1865,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
+          <t>Hackathon - Accelerate Developer Productivity</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2025-05-22 01:13:15 +0530</t>
+          <t>2025-05-22 10:37:15 +0530</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -1890,17 +1890,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>fabric-database-mirroring</t>
+          <t>Lunch and Learn: Developing a Multimodal RAG Solution</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2025-05-21 16:09:18 +0530</t>
+          <t>2025-05-22 01:13:15 +0530</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -1915,17 +1915,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
+          <t>fabric-database-mirroring</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2025-05-21 11:46:24 +0530</t>
+          <t>2025-05-21 16:09:18 +0530</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1940,17 +1940,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Innovate-with-AI</t>
+          <t xml:space="preserve">Build Intelligent Apps with Microsoft's Copilot stack &amp; Azure OpenAI  </t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2025-05-20 17:59:23 +0530</t>
+          <t>2025-05-21 11:46:24 +0530</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1965,17 +1965,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Infrastructure and Application Security</t>
+          <t>Innovate-with-AI</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2025-05-20 15:15:16 +0530</t>
+          <t>2025-05-20 17:59:23 +0530</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1990,17 +1990,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Implement CI-CD with GitHub Actions</t>
+          <t>Infrastructure and Application Security</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2025-05-19 14:20:37 +0530</t>
+          <t>2025-05-20 15:15:16 +0530</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 15:17:16 UTC</t>
+          <t>2025-06-13 15:19:23 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Sun Jun 15 01:27:58 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-13 15:19:23 UTC</t>
+          <t>2025-06-15 01:27:58 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Sun Jun 22 01:27:01 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-15 01:27:58 UTC</t>
+          <t>2025-06-22 01:27:01 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Sun Jun 29 01:36:54 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-22 01:27:01 UTC</t>
+          <t>2025-06-29 01:36:54 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Sun Jul  6 01:27:37 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-29 01:36:54 UTC</t>
+          <t>2025-07-06 01:27:37 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Sun Jul 13 01:39:09 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-07-06 01:27:37 UTC</t>
+          <t>2025-07-13 01:39:09 UTC</t>
         </is>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
     </row>

</xml_diff>